<commit_message>
update tab bom lenh san xuat
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
+++ b/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FORLIFE\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Forlife\code\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\data\xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE56D1A-19A3-4840-9A38-AACC3E9B7D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0475A948-3872-49A4-81B1-F619899481A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,6 +26,46 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>FORLIFE</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{59B4DBA0-2A6E-4D56-9559-9F5022AD467A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>FORLIFE:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FORLIFE:
+A/C nhập bộ phận sản xuất theo quy tắc sau:
+Nếu là 'Hàng tự sản xuất' thì nhập tu_san_xuat
+Bộ phận sản xuất gồm có những giá trị sau:
+('tu_san_xuat', 'Hàng tự sản xuất')
+('tp', 'Gia công TP')
+('npl', 'Gia công NPL')</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>admin</author>
@@ -681,11 +721,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,6 +920,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -888,7 +929,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,6 +1156,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix import lenh san xuat
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
+++ b/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Forlife\code\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\data\xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0475A948-3872-49A4-81B1-F619899481A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE90E73-49F0-4720-B954-9C0EDF5CACC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sản phẩm hoàn thành" sheetId="1" r:id="rId1"/>
     <sheet name="BOM" sheetId="3" r:id="rId2"/>
+    <sheet name="Chi phí" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -101,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
   <si>
     <t>Tên lệnh sản xuất</t>
   </si>
@@ -225,16 +226,36 @@
   </si>
   <si>
     <t>tu_san_xuat</t>
+  </si>
+  <si>
+    <t>Mã phí</t>
+  </si>
+  <si>
+    <t>Số lượng sản xất</t>
+  </si>
+  <si>
+    <t>Định mức (VND)</t>
+  </si>
+  <si>
+    <t>Tổng nhu cầu (VND)</t>
+  </si>
+  <si>
+    <t>622_NCNB</t>
+  </si>
+  <si>
+    <t>642_CPC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,8 +330,23 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,8 +375,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -363,14 +404,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
@@ -405,8 +463,14 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
+    <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
+    <cellStyle name="Comma" xfId="4" builtinId="3"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -724,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +993,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,4 +1223,66 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B37E9D6-9C3B-444F-A145-F09B13187BCA}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="18">
+        <v>500</v>
+      </c>
+      <c r="C2" s="18">
+        <v>2000</v>
+      </c>
+      <c r="D2" s="19">
+        <f>C2*B2</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="18">
+        <v>500</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19">
+        <v>3000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update import lenh san xuat
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
+++ b/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Forlife\code\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\data\xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE90E73-49F0-4720-B954-9C0EDF5CACC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF502BB-CE70-4C23-B37D-85E4002BEB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30540" yWindow="1365" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sản phẩm hoàn thành" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
     <author>admin</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>Tên lệnh sản xuất</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>642_CPC</t>
+  </si>
+  <si>
+    <t>NPL thay thế</t>
   </si>
 </sst>
 </file>
@@ -428,24 +431,28 @@
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -460,13 +467,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
-    <xf numFmtId="165" fontId="12" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
@@ -786,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,307 +917,251 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1111000000</v>
-      </c>
-      <c r="F5">
-        <v>1111000000</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="3">
-        <v>45108</v>
-      </c>
-      <c r="I5" s="3">
-        <v>45138</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="5"/>
-      <c r="J6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7">
-        <v>100</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" location="id=739&amp;model=account.analytic.account" display="https://dtbh.forlife.vn/web - id=739&amp;model=account.analytic.account" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E5" r:id="rId2" location="id=739&amp;model=account.analytic.account" display="https://dtbh.forlife.vn/web - id=739&amp;model=account.analytic.account" xr:uid="{27A0594E-A5D0-4A7C-BC9B-329BB878304F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="1" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="14">
+      <c r="G2" s="18">
         <v>0.51400000000000001</v>
       </c>
-      <c r="G2" s="12">
+      <c r="H2" s="16">
         <v>0.38</v>
       </c>
-      <c r="H2" s="13">
+      <c r="I2" s="17">
         <v>1.02</v>
       </c>
-      <c r="I2" s="15">
+      <c r="J2" s="7">
         <v>100</v>
       </c>
-      <c r="J2" s="15">
-        <f t="shared" ref="J2:J7" si="0">G2*H2*F2*I2</f>
+      <c r="K2" s="7">
+        <f t="shared" ref="K2:K7" si="0">H2*I2*G2*J2</f>
         <v>19.922640000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="13">
+      <c r="G3" s="17">
         <v>0.50700000000000001</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="16">
         <v>0.38</v>
       </c>
-      <c r="H3" s="13">
+      <c r="I3" s="17">
         <v>1.02</v>
       </c>
-      <c r="I3" s="15">
+      <c r="J3" s="7">
         <v>300</v>
       </c>
-      <c r="J3" s="15">
+      <c r="K3" s="7">
         <f t="shared" si="0"/>
         <v>58.953960000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="13">
+      <c r="G4" s="17">
         <v>0.53300000000000003</v>
       </c>
-      <c r="G4" s="12">
+      <c r="H4" s="16">
         <v>0.41</v>
       </c>
-      <c r="H4" s="13">
+      <c r="I4" s="17">
         <v>1.02</v>
       </c>
-      <c r="I4" s="15">
+      <c r="J4" s="7">
         <v>100</v>
       </c>
-      <c r="J4" s="15">
+      <c r="K4" s="7">
         <f t="shared" si="0"/>
         <v>22.29006</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="13">
+      <c r="G5" s="17">
         <v>0.53300000000000003</v>
       </c>
-      <c r="G5" s="12">
+      <c r="H5" s="16">
         <v>0.41</v>
       </c>
-      <c r="H5" s="13">
+      <c r="I5" s="17">
         <v>1.02</v>
       </c>
-      <c r="I5" s="15">
+      <c r="J5" s="7">
         <v>200</v>
       </c>
-      <c r="J5" s="15">
+      <c r="K5" s="7">
         <f t="shared" si="0"/>
         <v>44.580120000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="13">
+      <c r="G6" s="17">
         <v>0.53300000000000003</v>
       </c>
-      <c r="G6" s="12">
+      <c r="H6" s="16">
         <v>0.41</v>
       </c>
-      <c r="H6" s="13">
+      <c r="I6" s="17">
         <v>1.02</v>
       </c>
-      <c r="I6" s="15">
+      <c r="J6" s="7">
         <v>100</v>
       </c>
-      <c r="J6" s="15">
+      <c r="K6" s="7">
         <f t="shared" si="0"/>
         <v>22.29006</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="13">
+      <c r="G7" s="17">
         <v>0.498</v>
       </c>
-      <c r="G7" s="12">
+      <c r="H7" s="16">
         <v>0.41</v>
       </c>
-      <c r="H7" s="13">
+      <c r="I7" s="17">
         <v>1.02</v>
       </c>
-      <c r="I7" s="15">
+      <c r="J7" s="7">
         <v>400</v>
       </c>
-      <c r="J7" s="15">
+      <c r="K7" s="7">
         <f t="shared" si="0"/>
         <v>83.305440000000004</v>
       </c>
@@ -1230,7 +1178,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,43 +1190,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="10">
         <v>500</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="10">
         <v>2000</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="11">
         <f>C2*B2</f>
         <v>1000000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="10">
         <v>500</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19">
+      <c r="C3" s="10"/>
+      <c r="D3" s="11">
         <v>3000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update lenh san xuat
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
+++ b/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Forlife\code\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\data\xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087E3137-E5DB-4856-818D-D781BB9702D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297EF4F5-DDA0-4052-91C5-E8EFE1AC0EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sản phẩm hoàn thành" sheetId="1" r:id="rId1"/>
@@ -66,43 +66,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>admin</author>
-  </authors>
-  <commentList>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Cột này hệ thống phải tự tính khi người dùng import lên 
-= Cột ĐM *%Hao Hụt*HSQD*Số lượng sản xuất</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Tên lệnh sản xuất</t>
   </si>
@@ -175,9 +140,6 @@
   </si>
   <si>
     <t xml:space="preserve">Số lượng sản xuất </t>
-  </si>
-  <si>
-    <t>Tổng nhu cầu</t>
   </si>
   <si>
     <t>TEM-TK307-8373</t>
@@ -769,7 +731,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I2" sqref="I2:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +771,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>7</v>
@@ -832,7 +794,7 @@
         <v>1111000000</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1">
         <v>45108</v>
@@ -869,10 +831,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
         <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
       </c>
       <c r="C5" s="2">
         <v>1111000000</v>
@@ -881,7 +843,7 @@
         <v>1111000000</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>45108</v>
@@ -920,11 +882,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,21 +902,20 @@
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>13</v>
@@ -977,23 +938,20 @@
       <c r="K1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
@@ -1011,20 +969,16 @@
       <c r="K2" s="3">
         <v>200</v>
       </c>
-      <c r="L2" s="3">
-        <f t="shared" ref="L2:L4" si="0">I2*J2*H2*K2</f>
-        <v>44.580120000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
@@ -1042,12 +996,8 @@
       <c r="K3" s="3">
         <v>100</v>
       </c>
-      <c r="L3" s="3">
-        <f t="shared" si="0"/>
-        <v>22.29006</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>17</v>
@@ -1071,24 +1021,20 @@
       <c r="K4" s="3">
         <v>400</v>
       </c>
-      <c r="L4" s="3">
-        <f t="shared" si="0"/>
-        <v>83.305440000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
@@ -1106,20 +1052,16 @@
       <c r="K5" s="3">
         <v>200</v>
       </c>
-      <c r="L5" s="3">
-        <f t="shared" ref="L5:L7" si="1">I5*J5*H5*K5</f>
-        <v>44.580120000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
@@ -1137,12 +1079,8 @@
       <c r="K6" s="3">
         <v>100</v>
       </c>
-      <c r="L6" s="3">
-        <f t="shared" si="1"/>
-        <v>22.29006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>17</v>
@@ -1166,15 +1104,10 @@
       <c r="K7" s="3">
         <v>400</v>
       </c>
-      <c r="L7" s="3">
-        <f t="shared" si="1"/>
-        <v>83.305440000000004</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1198,22 +1131,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>31</v>
-      </c>
       <c r="F1" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1221,7 +1154,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4">
         <v>500</v>
@@ -1238,7 +1171,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4">
         <v>500</v>
@@ -1251,10 +1184,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4">
         <v>500</v>
@@ -1271,7 +1204,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="4">
         <v>500</v>

</xml_diff>

<commit_message>
fix code vietinbank, lenh san xuat
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
+++ b/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Forlife\code\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\data\xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297EF4F5-DDA0-4052-91C5-E8EFE1AC0EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8B52BE-C1F5-4ACF-BDCA-8E0EE6A2175B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,9 +123,6 @@
     <t>DTB-11-1711</t>
   </si>
   <si>
-    <t>Mã vật tư</t>
-  </si>
-  <si>
     <t xml:space="preserve">Đvt Lệnh sản xuất </t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>642_CPC</t>
   </si>
   <si>
-    <t>NPL thay thế</t>
-  </si>
-  <si>
     <t>Mã thành phẩm</t>
   </si>
   <si>
@@ -191,6 +185,12 @@
   </si>
   <si>
     <t>Lệnh sản xuất 1507_1</t>
+  </si>
+  <si>
+    <t>Mã vật tư(Mã vạch/Mã kĩ thuật)</t>
+  </si>
+  <si>
+    <t>NPL thay thế(Mã vạch/Mã kĩ thuật)</t>
   </si>
 </sst>
 </file>
@@ -771,7 +771,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>7</v>
@@ -794,7 +794,7 @@
         <v>1111000000</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1">
         <v>45108</v>
@@ -831,10 +831,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2">
         <v>1111000000</v>
@@ -843,7 +843,7 @@
         <v>1111000000</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1">
         <v>45108</v>
@@ -886,17 +886,17 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
@@ -906,16 +906,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>13</v>
@@ -924,19 +924,19 @@
         <v>14</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="J1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>22</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -944,14 +944,14 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
@@ -973,12 +973,12 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
@@ -1024,17 +1024,17 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
@@ -1056,12 +1056,12 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
@@ -1131,22 +1131,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="F1" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4">
         <v>500</v>
@@ -1171,7 +1171,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4">
         <v>500</v>
@@ -1184,10 +1184,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4">
         <v>500</v>
@@ -1204,7 +1204,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4">
         <v>500</v>

</xml_diff>

<commit_message>
add code sinh ma vu viec theo rule
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
+++ b/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Forlife\code\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\data\xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8B52BE-C1F5-4ACF-BDCA-8E0EE6A2175B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D8C97F-56A0-4E6D-8EF0-F2AB3F8D7D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -886,7 +886,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +964,7 @@
         <v>0.41</v>
       </c>
       <c r="J2" s="8">
-        <v>1.02</v>
+        <v>1</v>
       </c>
       <c r="K2" s="3">
         <v>200</v>
@@ -991,7 +991,7 @@
         <v>0.41</v>
       </c>
       <c r="J3" s="8">
-        <v>1.02</v>
+        <v>2</v>
       </c>
       <c r="K3" s="3">
         <v>100</v>
@@ -1016,7 +1016,7 @@
         <v>0.41</v>
       </c>
       <c r="J4" s="8">
-        <v>1.02</v>
+        <v>1</v>
       </c>
       <c r="K4" s="3">
         <v>400</v>
@@ -1047,7 +1047,7 @@
         <v>0.41</v>
       </c>
       <c r="J5" s="8">
-        <v>1.02</v>
+        <v>2</v>
       </c>
       <c r="K5" s="3">
         <v>200</v>
@@ -1074,7 +1074,7 @@
         <v>0.41</v>
       </c>
       <c r="J6" s="8">
-        <v>1.02</v>
+        <v>1</v>
       </c>
       <c r="K6" s="3">
         <v>100</v>
@@ -1099,7 +1099,7 @@
         <v>0.41</v>
       </c>
       <c r="J7" s="8">
-        <v>1.02</v>
+        <v>2</v>
       </c>
       <c r="K7" s="3">
         <v>400</v>

</xml_diff>

<commit_message>
fix label template import lsx
update import lenh san xuat

update import lenh san xuat
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
+++ b/addons/custom/forlife_purchase/data/xml/template_lsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Forlife\code\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\data\xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D8C97F-56A0-4E6D-8EF0-F2AB3F8D7D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3790573-A07C-469A-BF4D-90E06F7E3AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sản phẩm hoàn thành" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>Tên lệnh sản xuất</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Bộ phận quản lý</t>
-  </si>
-  <si>
-    <t>Bộ phận sản xuất</t>
   </si>
   <si>
     <t>Dự kiến sản xuất từ</t>
@@ -191,6 +188,18 @@
   </si>
   <si>
     <t>NPL thay thế(Mã vạch/Mã kĩ thuật)</t>
+  </si>
+  <si>
+    <t>Nhãn hàng</t>
+  </si>
+  <si>
+    <t>Quản lý đơn hàng</t>
+  </si>
+  <si>
+    <t>Đối tượng gia công</t>
+  </si>
+  <si>
+    <t>Phân loại sản xuất</t>
   </si>
 </sst>
 </file>
@@ -728,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,11 +753,13 @@
     <col min="6" max="6" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="11" width="17.42578125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -762,30 +773,39 @@
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="14" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="2">
         <v>1111000000</v>
@@ -794,7 +814,7 @@
         <v>1111000000</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1">
         <v>45108</v>
@@ -805,36 +825,38 @@
       <c r="H2" s="10">
         <v>100000</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="L3" t="s">
         <v>11</v>
       </c>
-      <c r="J2">
+      <c r="M3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
       </c>
       <c r="C5" s="2">
         <v>1111000000</v>
@@ -843,7 +865,7 @@
         <v>1111000000</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1">
         <v>45108</v>
@@ -854,19 +876,21 @@
       <c r="H5" s="10">
         <v>100000</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="L6" t="s">
         <v>11</v>
       </c>
-      <c r="J5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="2"/>
-      <c r="I6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6">
+      <c r="M6">
         <v>200</v>
       </c>
     </row>
@@ -885,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -906,56 +930,56 @@
   <sheetData>
     <row r="1" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>40</v>
-      </c>
       <c r="E1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>14</v>
-      </c>
       <c r="G1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="J1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>21</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="8">
         <v>0.53300000000000003</v>
@@ -973,16 +997,16 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="8">
         <v>0.53300000000000003</v>
@@ -1000,14 +1024,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="8">
         <v>0.498</v>
@@ -1024,21 +1048,21 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="8">
         <v>0.53300000000000003</v>
@@ -1056,16 +1080,16 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="8">
         <v>0.53300000000000003</v>
@@ -1083,14 +1107,14 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" s="8">
         <v>0.498</v>
@@ -1131,30 +1155,30 @@
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>29</v>
-      </c>
       <c r="F1" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4">
         <v>500</v>
@@ -1171,7 +1195,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4">
         <v>500</v>
@@ -1184,10 +1208,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4">
         <v>500</v>
@@ -1204,7 +1228,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="4">
         <v>500</v>

</xml_diff>